<commit_message>
renamed unipept etnp excel ss
</commit_message>
<xml_diff>
--- a/analyses/lee-1984-etnp-pAA.xlsx
+++ b/analyses/lee-1984-etnp-pAA.xlsx
@@ -170,7 +170,7 @@
     <numFmt numFmtId="166" formatCode="#,##0"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -233,19 +233,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -289,7 +276,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -306,11 +293,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -386,7 +369,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -568,11 +551,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="35455064"/>
-        <c:axId val="54200906"/>
+        <c:axId val="80756011"/>
+        <c:axId val="38895404"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="35455064"/>
+        <c:axId val="80756011"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -604,12 +587,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54200906"/>
+        <c:crossAx val="38895404"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54200906"/>
+        <c:axId val="38895404"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="2100"/>
@@ -643,7 +626,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35455064"/>
+        <c:crossAx val="80756011"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -671,7 +654,293 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Mol % lysine in suspended particulate amino acid pool</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"Mol % lysine in suspended particulate amino acid pool"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mol % lysine in suspended particulate amino acid pool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="806000"/>
+            </a:solidFill>
+            <a:ln w="15840">
+              <a:solidFill>
+                <a:srgbClr val="806000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="806000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'VERTEX-II SUS'!$B$41:$K$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0493975903614458</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.104081632653061</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.076</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.03125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0408163265306122</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'VERTEX-II SUS'!$B$6:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="78763461"/>
+        <c:axId val="6890597"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="78763461"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="6890597"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="6890597"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="2100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="78763461"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -853,11 +1122,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="21369146"/>
-        <c:axId val="98489369"/>
+        <c:axId val="48754953"/>
+        <c:axId val="11501337"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="21369146"/>
+        <c:axId val="48754953"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,12 +1158,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98489369"/>
+        <c:crossAx val="11501337"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98489369"/>
+        <c:axId val="11501337"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="2100"/>
@@ -928,7 +1197,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21369146"/>
+        <c:crossAx val="48754953"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -956,7 +1225,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1138,11 +1407,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="16456390"/>
-        <c:axId val="20229093"/>
+        <c:axId val="27051641"/>
+        <c:axId val="24407934"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16456390"/>
+        <c:axId val="27051641"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,12 +1443,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20229093"/>
+        <c:crossAx val="24407934"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20229093"/>
+        <c:axId val="24407934"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="2100"/>
@@ -1213,7 +1482,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16456390"/>
+        <c:crossAx val="27051641"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
@@ -1242,7 +1511,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1424,11 +1693,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="17958741"/>
-        <c:axId val="23425437"/>
+        <c:axId val="55525356"/>
+        <c:axId val="89766883"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="17958741"/>
+        <c:axId val="55525356"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1460,12 +1729,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23425437"/>
+        <c:crossAx val="89766883"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="23425437"/>
+        <c:axId val="89766883"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="2100"/>
@@ -1499,7 +1768,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17958741"/>
+        <c:crossAx val="55525356"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
@@ -1528,7 +1797,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1710,11 +1979,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="63717225"/>
-        <c:axId val="68538379"/>
+        <c:axId val="40132130"/>
+        <c:axId val="56714761"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63717225"/>
+        <c:axId val="40132130"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1746,12 +2015,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68538379"/>
+        <c:crossAx val="56714761"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68538379"/>
+        <c:axId val="56714761"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="2100"/>
@@ -1785,7 +2054,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63717225"/>
+        <c:crossAx val="40132130"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
@@ -1814,7 +2083,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1996,11 +2265,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="63691157"/>
-        <c:axId val="44336619"/>
+        <c:axId val="78344678"/>
+        <c:axId val="75833029"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63691157"/>
+        <c:axId val="78344678"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2032,12 +2301,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44336619"/>
+        <c:crossAx val="75833029"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44336619"/>
+        <c:axId val="75833029"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="2100"/>
@@ -2071,7 +2340,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63691157"/>
+        <c:crossAx val="78344678"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
@@ -2100,7 +2369,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3938,11 +4207,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="81734598"/>
-        <c:axId val="11491698"/>
+        <c:axId val="26101275"/>
+        <c:axId val="16212549"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81734598"/>
+        <c:axId val="26101275"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3974,12 +4243,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11491698"/>
+        <c:crossAx val="16212549"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="11491698"/>
+        <c:axId val="16212549"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="2000"/>
@@ -4012,7 +4281,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81734598"/>
+        <c:crossAx val="26101275"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4064,7 +4333,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4384,11 +4653,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="80705093"/>
-        <c:axId val="70412531"/>
+        <c:axId val="65095591"/>
+        <c:axId val="80523532"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80705093"/>
+        <c:axId val="65095591"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4420,12 +4689,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70412531"/>
+        <c:crossAx val="80523532"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70412531"/>
+        <c:axId val="80523532"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="2100"/>
@@ -4459,7 +4728,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80705093"/>
+        <c:crossAx val="65095591"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
@@ -4488,7 +4757,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4670,11 +4939,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="93687235"/>
-        <c:axId val="84340622"/>
+        <c:axId val="95242369"/>
+        <c:axId val="5315460"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93687235"/>
+        <c:axId val="95242369"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4706,12 +4975,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84340622"/>
+        <c:crossAx val="5315460"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84340622"/>
+        <c:axId val="5315460"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="2100"/>
@@ -4745,293 +5014,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93687235"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="100"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Mol % lysine in suspended particulate amino acid pool</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>"Mol % lysine in suspended particulate amino acid pool"</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mol % lysine in suspended particulate amino acid pool</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="806000"/>
-            </a:solidFill>
-            <a:ln w="15840">
-              <a:solidFill>
-                <a:srgbClr val="806000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="806000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'VERTEX-II SUS'!$B$41:$K$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0444444444444444</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0493975903614458</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.104081632653061</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0888888888888889</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.076</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.03125</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0125</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.00666666666666667</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0408163265306122</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'VERTEX-II SUS'!$B$6:$K$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1250</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="97204026"/>
-        <c:axId val="46108250"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="97204026"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="46108250"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="46108250"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-          <c:max val="2100"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="97204026"/>
+        <c:crossAx val="95242369"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
@@ -5071,9 +5054,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>672840</xdr:colOff>
+      <xdr:colOff>672480</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:rowOff>125640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5081,8 +5064,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13152960" y="749160"/>
-        <a:ext cx="4379760" cy="7530120"/>
+        <a:off x="13157640" y="749160"/>
+        <a:ext cx="4381560" cy="7529760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5101,9 +5084,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>380520</xdr:colOff>
+      <xdr:colOff>380160</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5111,8 +5094,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17943840" y="774720"/>
-        <a:ext cx="4398480" cy="7517520"/>
+        <a:off x="17951400" y="774720"/>
+        <a:ext cx="4401000" cy="7517160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5131,9 +5114,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>240840</xdr:colOff>
+      <xdr:colOff>240480</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5141,8 +5124,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="22711320" y="825480"/>
-        <a:ext cx="4593600" cy="7517880"/>
+        <a:off x="22721760" y="825480"/>
+        <a:ext cx="4596120" cy="7517520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5161,9 +5144,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>316800</xdr:colOff>
+      <xdr:colOff>316440</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5171,8 +5154,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28084680" y="812880"/>
-        <a:ext cx="4398480" cy="7517880"/>
+        <a:off x="28098720" y="812880"/>
+        <a:ext cx="4400640" cy="7517520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5191,9 +5174,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>316800</xdr:colOff>
+      <xdr:colOff>316440</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5201,8 +5184,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33186960" y="812880"/>
-        <a:ext cx="4398480" cy="7517880"/>
+        <a:off x="33203880" y="812880"/>
+        <a:ext cx="4401000" cy="7517520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5221,9 +5204,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>317160</xdr:colOff>
+      <xdr:colOff>316800</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5231,8 +5214,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="38289240" y="812880"/>
-        <a:ext cx="4398840" cy="7517880"/>
+        <a:off x="38309760" y="812880"/>
+        <a:ext cx="4400640" cy="7517520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5251,9 +5234,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>24840</xdr:colOff>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5261,8 +5244,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13159080" y="8299440"/>
-        <a:ext cx="11889000" cy="5682240"/>
+        <a:off x="13163760" y="8299440"/>
+        <a:ext cx="11896200" cy="5681880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5281,9 +5264,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
-      <xdr:colOff>317160</xdr:colOff>
+      <xdr:colOff>316800</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5291,8 +5274,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="43391520" y="812880"/>
-        <a:ext cx="4398840" cy="7517880"/>
+        <a:off x="43415280" y="812880"/>
+        <a:ext cx="4400640" cy="7517520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5311,9 +5294,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>317160</xdr:colOff>
+      <xdr:colOff>316800</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5321,8 +5304,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="48493800" y="812880"/>
-        <a:ext cx="4398480" cy="7517880"/>
+        <a:off x="48520440" y="812880"/>
+        <a:ext cx="4401000" cy="7517520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5341,9 +5324,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>55</xdr:col>
-      <xdr:colOff>317160</xdr:colOff>
+      <xdr:colOff>316800</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>177480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5351,8 +5334,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="53596080" y="812880"/>
-        <a:ext cx="4398480" cy="7517880"/>
+        <a:off x="53625960" y="812880"/>
+        <a:ext cx="4400640" cy="7517520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5376,7 +5359,7 @@
       <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.66"/>
@@ -6837,7 +6820,7 @@
       <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.85"/>
   </cols>
@@ -7400,7 +7383,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>